<commit_message>
+ 新增 mp_staff_second_file_type 员工附件二级分类表
</commit_message>
<xml_diff>
--- a/doc/核心人力表结构NEW-20200910.xlsx
+++ b/doc/核心人力表结构NEW-20200910.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24300" windowHeight="10590" activeTab="2"/>
+    <workbookView windowWidth="21000" windowHeight="9090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="规则必看！！！" sheetId="7" r:id="rId1"/>
@@ -14039,14 +14039,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -14068,6 +14068,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
@@ -14076,7 +14091,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -14090,27 +14113,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -14137,6 +14144,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -14153,25 +14168,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -14202,55 +14202,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -14268,13 +14250,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -14286,7 +14334,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -14304,31 +14370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -14341,48 +14383,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -14493,6 +14493,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -14509,24 +14524,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -14542,6 +14553,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -14569,36 +14589,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -14607,37 +14607,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -14646,94 +14640,100 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -18562,7 +18562,7 @@
   <dimension ref="A1:Q193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D169" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175:H175"/>
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -24722,7 +24722,7 @@
     </row>
     <row r="181" spans="6:17">
       <c r="F181" s="6" t="s">
-        <v>61</v>
+        <v>207</v>
       </c>
       <c r="G181" s="6" t="s">
         <v>918</v>
@@ -24774,7 +24774,7 @@
     </row>
     <row r="183" spans="6:17">
       <c r="F183" s="6" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="G183" s="6" t="s">
         <v>918</v>

</xml_diff>